<commit_message>
docs/edit: adding the edited document (work log) – Lopizzo Maximilian.
</commit_message>
<xml_diff>
--- a/docs/worklogs/Maximilian_Lopizzo_worklog.xlsx
+++ b/docs/worklogs/Maximilian_Lopizzo_worklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alopi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A7ACAE-9900-457E-B869-76E6AAD38230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37990BF5-2C0F-4A81-A469-C2DBBA2EA097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16371" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
   <si>
     <t>Jour</t>
   </si>
@@ -142,6 +142,44 @@
   <si>
     <t>Soudure du veroBoard pour le transformateur (9v -&gt; 5v stable), passage des câbles et découpe de ces derniers à la bonne taille, fixation de l'alimentation 9v à l'arrière du véhicule</t>
   </si>
+  <si>
+    <t>mercredi, 21 janvier 2026</t>
+  </si>
+  <si>
+    <t>jeudi, 22 janvier 2026</t>
+  </si>
+  <si>
+    <t>Démontage des connecteurs Dupont et soudure sur les câbles des divers éléments prévus pour l’ESP</t>
+  </si>
+  <si>
+    <t>Test de fonctionnement des LED avec télécommande sur le véhicule</t>
+  </si>
+  <si>
+    <t>Soudure et montage du veroboard pour le moteur avant du véhicule, ainsi que tests basiques de fonctionnement</t>
+  </si>
+  <si>
+    <t>Donné du travail au CFC 1ʳᵉ année et aide à la résolution des problèmes rencontrés</t>
+  </si>
+  <si>
+    <t>Terminaison des connecteurs Dupont et ajout de pins sur le micro-transformateur (9 → 6 V)</t>
+  </si>
+  <si>
+    <t>Analyse de divers problèmes connus sur le véhicule et modification de ces derniers (recâblage d’une partie du véhicule pour un meilleur contrôle, préparation d’un veroboard pour les LED avant)</t>
+  </si>
+  <si>
+    <t>Test de fonctionnement du moteur avec LED et télécommande</t>
+  </si>
+  <si>
+    <t>Recherche sur le problème concernant le moteur électrique gérant le déplacement du véhicule et la batterie lithium-ion trop grande + donné du travail à Tristan et aide à la soudure du nouveau connecteur pour la batterie</t>
+  </si>
+  <si>
+    <t>Réparation du système de direction (avec la force du moteur, la direction réalisée avec des fils n’a pas supporté la tension et la force appliquées ; il a fallu refaire tout le système)</t>
+  </si>
+  <si>
+    <t>Suite à un problème dû au transformateur réalisé, les piles n’ont pas supporté la charge du moteur, et il a fallu un bon moment pour comprendre d’où venait le problème.
+De plus, à cause d’une mauvaise gestion des composants électroniques et d’une recherche insuffisante, beaucoup de temps a été perdu à chercher un module permettant une chute de tension stable.
+Au final, ce module n’a jamais été utilisé : nous avons simplement acheté de nouvelles piles.</t>
+  </si>
 </sst>
 </file>
 
@@ -213,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -276,6 +314,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -894,19 +935,19 @@
                   <c:v>3.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.5</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.25</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1927,8 +1968,8 @@
   <dimension ref="A1:F500"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.35"/>
@@ -2215,76 +2256,168 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="8"/>
+    <row r="16" spans="1:6" ht="30.9" x14ac:dyDescent="0.35">
+      <c r="A16" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="14">
+        <v>2</v>
+      </c>
+      <c r="C16" s="11">
+        <v>2.5</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="F16" s="8"/>
     </row>
     <row r="17" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="14">
+        <v>2</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>37</v>
+      </c>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="8"/>
+    <row r="18" spans="1:6" ht="30.9" x14ac:dyDescent="0.35">
+      <c r="A18" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="14">
+        <v>2</v>
+      </c>
+      <c r="C18" s="11">
+        <v>1</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="8"/>
+    <row r="19" spans="1:6" ht="30.9" x14ac:dyDescent="0.35">
+      <c r="A19" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="14">
+        <v>2</v>
+      </c>
+      <c r="C19" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>39</v>
+      </c>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="8"/>
+    <row r="20" spans="1:6" ht="30.9" x14ac:dyDescent="0.35">
+      <c r="A20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="14">
+        <v>2</v>
+      </c>
+      <c r="C20" s="11">
+        <v>2</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>40</v>
+      </c>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="8"/>
+    <row r="21" spans="1:6" ht="46.3" x14ac:dyDescent="0.35">
+      <c r="A21" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="14">
+        <v>2</v>
+      </c>
+      <c r="C21" s="11">
+        <v>1.75</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="20"/>
+    </row>
+    <row r="22" spans="1:6" ht="123.45" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="14">
+        <v>2</v>
+      </c>
+      <c r="C22" s="11">
+        <v>1.5</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="61.75" x14ac:dyDescent="0.35">
+      <c r="A23" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="14">
+        <v>2</v>
+      </c>
+      <c r="C23" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="20" t="s">
+        <v>43</v>
+      </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="8"/>
+    <row r="24" spans="1:6" ht="46.3" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="14">
+        <v>2</v>
+      </c>
+      <c r="C24" s="11">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>44</v>
+      </c>
       <c r="F24" s="8"/>
     </row>
     <row r="25" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -6168,7 +6301,7 @@
       </c>
       <c r="B3" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>3.5</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -6177,7 +6310,7 @@
       </c>
       <c r="B4" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>9.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -6186,7 +6319,7 @@
       </c>
       <c r="B5" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>0.25</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -6204,7 +6337,7 @@
       </c>
       <c r="B7" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>2.25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
doc: update report and worklog and add PDF version
</commit_message>
<xml_diff>
--- a/docs/worklogs/Maximilian_Lopizzo_worklog.xlsx
+++ b/docs/worklogs/Maximilian_Lopizzo_worklog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alopi\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FCF47E-1501-4C5C-8162-D4F1A78CF26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2A3C41A-99CD-4878-AAF2-E84E815515C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16371" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="68">
   <si>
     <t>Jour</t>
   </si>
@@ -238,6 +238,15 @@
   <si>
     <t>Tests du contrôleur moteur, du freinage d’urgence et du mode automatique</t>
   </si>
+  <si>
+    <t>vendredi, 30 janvier 2026</t>
+  </si>
+  <si>
+    <t>Animation des portes ouvertes et présentation du Pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Débrief avec l'équipe </t>
+  </si>
 </sst>
 </file>
 
@@ -309,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -385,24 +394,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1038,7 +1029,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.25</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2052,9 +2043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="116" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.6" x14ac:dyDescent="0.35"/>
@@ -2634,7 +2625,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B32" s="14">
@@ -2646,13 +2637,13 @@
       <c r="D32" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="21" t="s">
         <v>60</v>
       </c>
       <c r="F32" s="8"/>
     </row>
     <row r="33" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B33" s="14">
@@ -2664,13 +2655,13 @@
       <c r="D33" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="27" t="s">
+      <c r="E33" s="21" t="s">
         <v>61</v>
       </c>
       <c r="F33" s="8"/>
     </row>
     <row r="34" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="28" t="s">
+      <c r="A34" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B34" s="14">
@@ -2682,13 +2673,13 @@
       <c r="D34" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="E34" s="21" t="s">
         <v>62</v>
       </c>
       <c r="F34" s="8"/>
     </row>
     <row r="35" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B35" s="14">
@@ -2700,13 +2691,13 @@
       <c r="D35" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="21" t="s">
         <v>63</v>
       </c>
       <c r="F35" s="8"/>
     </row>
     <row r="36" spans="1:6" ht="30.9" x14ac:dyDescent="0.35">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B36" s="14">
@@ -2724,7 +2715,7 @@
       <c r="F36" s="8"/>
     </row>
     <row r="37" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="30" t="s">
+      <c r="A37" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B37" s="14">
@@ -2736,25 +2727,45 @@
       <c r="D37" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E37" s="31" t="s">
+      <c r="E37" s="21" t="s">
         <v>59</v>
       </c>
       <c r="F37" s="8"/>
     </row>
     <row r="38" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="6"/>
-      <c r="B38" s="14"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="8"/>
+      <c r="A38" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="23">
+        <v>3</v>
+      </c>
+      <c r="C38" s="24">
+        <v>2</v>
+      </c>
+      <c r="D38" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>66</v>
+      </c>
       <c r="F38" s="8"/>
     </row>
     <row r="39" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
-      <c r="B39" s="14"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="8"/>
+      <c r="A39" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="23">
+        <v>3</v>
+      </c>
+      <c r="C39" s="24">
+        <v>1.75</v>
+      </c>
+      <c r="D39" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>67</v>
+      </c>
       <c r="F39" s="8"/>
     </row>
     <row r="40" spans="1:6" ht="25" customHeight="1" x14ac:dyDescent="0.35">
@@ -6472,7 +6483,7 @@
           <x14:formula1>
             <xm:f>Listes!$A:$A</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D26 D29:D300</xm:sqref>
+          <xm:sqref>D1:D26 D29:D37 D40:D300</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6572,7 +6583,7 @@
       </c>
       <c r="B9" s="11">
         <f>SUMIF(Journal!$D$2:$D$160,Tableau13[[#This Row],[Type]],Journal!$C$2:$C$160)</f>
-        <v>1.25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>